<commit_message>
define variables switch language
</commit_message>
<xml_diff>
--- a/config/languageFile.xlsx
+++ b/config/languageFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATEN\PHD\CAMtools_CAMEL\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05D99CFF-6FD7-4FE9-B530-D2734160B800}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D43200-CF54-4522-9EEB-33DEF697B261}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,24 @@
         </r>
       </text>
     </comment>
-    <comment ref="C50" authorId="1" shapeId="0" xr:uid="{A5E30C12-9A09-4005-AC0C-695CE60E1B9A}">
+    <comment ref="C30" authorId="0" shapeId="0" xr:uid="{951FEFAD-8A39-472C-B45E-1E8B581A6A94}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    I'm not sure whether "agreement or disagreement" might be an error here. I suppose it's more about the support or inhibion between concepts (that appear mentioned earlier in the table), right?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C54" authorId="1" shapeId="0" xr:uid="{A5E30C12-9A09-4005-AC0C-695CE60E1B9A}">
       <text>
         <r>
           <rPr>
@@ -65,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="239">
   <si>
     <t>english</t>
   </si>
@@ -160,9 +177,6 @@
     <t>&lt;b&gt;Update:&lt;/b&gt; Double click on existing concept</t>
   </si>
   <si>
-    <t>&lt;b&gt;Delete:&lt;/b&gt; Double click on existing concept and press on the “trash bin” symbol top right</t>
-  </si>
-  <si>
     <t>qr_concept_20</t>
   </si>
   <si>
@@ -199,9 +213,6 @@
     <t>&lt;b&gt;Change type and strength:&lt;/b&gt; Use the slider to change the emotional attribution and strength of the concept</t>
   </si>
   <si>
-    <t>&lt;b&gt;Add comment:&lt;/b&gt; type comment in the “Comment” section</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Create:&lt;/b&gt; Click on two concepts to draw a connection</t>
   </si>
   <si>
@@ -253,15 +264,6 @@
     <t xml:space="preserve">Clicking on the buttons in the upper bar leads to the following results: </t>
   </si>
   <si>
-    <t>save Cognitive Affective Map and send data to the server</t>
-  </si>
-  <si>
-    <t>download Cognitive Affective Map as a picture</t>
-  </si>
-  <si>
-    <t>delete Cognitive Affective Map and no data will be send to the server</t>
-  </si>
-  <si>
     <t>qr_buttons_11</t>
   </si>
   <si>
@@ -388,12 +390,6 @@
     <t>Concepts influence each other in a one-sided direction. Press button multiple times to change direction</t>
   </si>
   <si>
-    <t>cd_05</t>
-  </si>
-  <si>
-    <t>cd_06</t>
-  </si>
-  <si>
     <t>qr_top</t>
   </si>
   <si>
@@ -601,21 +597,6 @@
     <t>Hacer clic en los botones de la barra superior lleva a los siguientes resultados:</t>
   </si>
   <si>
-    <t>Cognitive Affective Map speichern und Daten zum Server senden</t>
-  </si>
-  <si>
-    <t>Guardar Cognitive Affective Map y mandar datos al servidor</t>
-  </si>
-  <si>
-    <t>Cognitive Affective Map als Bild herunterladen</t>
-  </si>
-  <si>
-    <t>Cognitive Affective Map löschen und keine Daten werden zum Server gesendet</t>
-  </si>
-  <si>
-    <t>Borrar Cognitive Affective Map y no se envian datos al servidor</t>
-  </si>
-  <si>
     <t>Legende</t>
   </si>
   <si>
@@ -655,9 +636,6 @@
     <t>Guardar CAM en formato de imagen</t>
   </si>
   <si>
-    <t xml:space="preserve">Bajar Cognitive Affective Map en de imagen </t>
-  </si>
-  <si>
     <t>CAM löschen</t>
   </si>
   <si>
@@ -734,6 +712,93 @@
   </si>
   <si>
     <t>Bitte wechseln oder minimieren Sie das Browserfenster nicht, während die Studie läuft, sondern nur, wenn es während der Studie eine Pause gibt.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Delete:&lt;/b&gt; Double click on existing concept and press on the "trash bin" symbol top right</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Add comment:&lt;/b&gt; type comment in the "Comment" section</t>
+  </si>
+  <si>
+    <t>qr_connection_21a</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Change strength:&lt;/b&gt; Use the slider to change the strength of the connection</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Stärke verändern:&lt;/b&gt; Benutzen Sie den Regler, um die Stärke der Verbindung zu verändern</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Cambiar intensidad:&lt;/b&gt; Use el control deslizante para cambiar el de la conexión (reforzamineto)</t>
+  </si>
+  <si>
+    <t>Delete Concept</t>
+  </si>
+  <si>
+    <t>Konzept löschen</t>
+  </si>
+  <si>
+    <t>Borrar concepto</t>
+  </si>
+  <si>
+    <t>cd_05button</t>
+  </si>
+  <si>
+    <t>cd_06button</t>
+  </si>
+  <si>
+    <t>Strength of Connection:</t>
+  </si>
+  <si>
+    <t>cd_07buttonDelete</t>
+  </si>
+  <si>
+    <t>Delete Connector</t>
+  </si>
+  <si>
+    <t>Verbindung löschen</t>
+  </si>
+  <si>
+    <t>Borrar conexión</t>
+  </si>
+  <si>
+    <t>nd_05buttonDelete</t>
+  </si>
+  <si>
+    <t>download Cognitive-Affective Map as a picture</t>
+  </si>
+  <si>
+    <t>delete Cognitive-Affective Map and no data will be send to the server</t>
+  </si>
+  <si>
+    <t>save Cognitive-Affective Map and send data to the server</t>
+  </si>
+  <si>
+    <t>Cognitive-Affective Map speichern und Daten zum Server senden</t>
+  </si>
+  <si>
+    <t>Cognitive-Affective Map als Bild herunterladen</t>
+  </si>
+  <si>
+    <t>Cognitive-Affective Map löschen und keine Daten werden zum Server gesendet</t>
+  </si>
+  <si>
+    <t>Borrar Cognitive-Affective Map y no se envian datos al servidor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bajar Cognitive-Affective Map en de imagen </t>
+  </si>
+  <si>
+    <t>Guardar Cognitive-Affective Map y mandar datos al servidor</t>
+  </si>
+  <si>
+    <t>cd_01a</t>
+  </si>
+  <si>
+    <t>Stärke der Verbindung:</t>
+  </si>
+  <si>
+    <t>Intensidad de la conexión</t>
   </si>
 </sst>
 </file>
@@ -749,12 +814,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -769,7 +840,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -778,6 +849,16 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1077,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,10 +1176,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1107,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -1121,36 +1202,36 @@
     </row>
     <row r="2" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>119</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -1158,33 +1239,33 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1198,10 +1279,10 @@
         <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1215,10 +1296,10 @@
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1232,10 +1313,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1249,10 +1330,10 @@
         <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1266,10 +1347,10 @@
         <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1283,10 +1364,10 @@
         <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1300,10 +1381,10 @@
         <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1317,44 +1398,44 @@
         <v>23</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1368,10 +1449,10 @@
         <v>25</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1385,10 +1466,10 @@
         <v>29</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1402,10 +1483,10 @@
         <v>30</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1416,608 +1497,676 @@
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>44</v>
+        <v>211</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="D32" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D33" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="B37" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>69</v>
+        <v>228</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>183</v>
+        <v>232</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>184</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="D43" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="B47" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="D49" s="2" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>103</v>
+        <v>226</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>220</v>
+        <v>96</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>105</v>
+        <v>236</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>102</v>
+        <v>221</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="B54" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>106</v>
+        <v>206</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>216</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
language file - correction
</commit_message>
<xml_diff>
--- a/config/languageFile.xlsx
+++ b/config/languageFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fenn\Nextcloud\Artikel Cognitive Affective Maps Tools\CAM tools\CAMtools_CAMEL\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E115F24-009F-43AD-9DDD-31118F51FF91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A170412D-D095-4CF4-B6D3-B684FA3DD5B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1324,9 +1324,6 @@
     <t>Veuillez connecter tous vos</t>
   </si>
   <si>
-    <t>différents groupes de concepts de votre Cognitive Affective Map.</t>
-  </si>
-  <si>
     <t>Vos données de la CAM ont été envoyées au serveur. Nous vous remercions de votre participation ! Vous allez être redirigé vers la fin ou la dernière partie de l'étude.</t>
   </si>
   <si>
@@ -1421,6 +1418,9 @@
   </si>
   <si>
     <t>chinese</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> différents groupes de concepts de votre Cognitive Affective Map.</t>
   </si>
 </sst>
 </file>
@@ -1766,8 +1766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1799,7 +1799,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H1" t="s">
         <v>57</v>
@@ -1902,7 +1902,7 @@
         <v>117</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>118</v>
@@ -2102,7 +2102,7 @@
         <v>134</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>135</v>
@@ -2182,7 +2182,7 @@
         <v>139</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>138</v>
@@ -2222,7 +2222,7 @@
         <v>159</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>143</v>
@@ -2262,7 +2262,7 @@
         <v>146</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>147</v>
@@ -2342,7 +2342,7 @@
         <v>157</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>158</v>
@@ -2362,7 +2362,7 @@
         <v>160</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>163</v>
@@ -2462,7 +2462,7 @@
         <v>169</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>170</v>
@@ -2702,7 +2702,7 @@
         <v>186</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>187</v>
@@ -2722,7 +2722,7 @@
         <v>188</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>189</v>
@@ -2822,7 +2822,7 @@
         <v>237</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>238</v>
@@ -3142,7 +3142,7 @@
         <v>267</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>413</v>
+        <v>445</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>332</v>
@@ -3162,7 +3162,7 @@
         <v>270</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>333</v>
@@ -3182,7 +3182,7 @@
         <v>272</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>334</v>
@@ -3202,7 +3202,7 @@
         <v>288</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>335</v>
@@ -3222,7 +3222,7 @@
         <v>289</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>336</v>
@@ -3242,7 +3242,7 @@
         <v>290</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>337</v>
@@ -3262,7 +3262,7 @@
         <v>291</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>338</v>
@@ -3282,7 +3282,7 @@
         <v>292</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>339</v>
@@ -3302,7 +3302,7 @@
         <v>293</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>340</v>
@@ -3322,7 +3322,7 @@
         <v>341</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>342</v>
@@ -3342,7 +3342,7 @@
         <v>303</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>339</v>
@@ -3363,7 +3363,7 @@
         <v>304</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>343</v>
@@ -3383,7 +3383,7 @@
         <v>305</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>344</v>
@@ -3403,7 +3403,7 @@
         <v>306</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>345</v>
@@ -3423,7 +3423,7 @@
         <v>346</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>347</v>
@@ -3443,7 +3443,7 @@
         <v>349</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>350</v>
@@ -3463,7 +3463,7 @@
         <v>351</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>352</v>
@@ -3483,7 +3483,7 @@
         <v>353</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>354</v>
@@ -3503,7 +3503,7 @@
         <v>355</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>356</v>
@@ -3523,7 +3523,7 @@
         <v>357</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>321</v>
@@ -3563,7 +3563,7 @@
         <v>361</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F89" s="3" t="s">
         <v>362</v>

</xml_diff>

<commit_message>
chinese language - 2 languages files (encoding)
</commit_message>
<xml_diff>
--- a/config/languageFile.xlsx
+++ b/config/languageFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fenn\Nextcloud\Artikel Cognitive Affective Maps Tools\CAM tools\CAMtools_CAMEL\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CBAC216-C8BE-4B60-AAE1-345A6FD181D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC1602C-A6AD-49F2-ABCC-027303E7C34B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2227,8 +2227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
oppose instead of Inhibition
</commit_message>
<xml_diff>
--- a/config/languageFile.xlsx
+++ b/config/languageFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fenn\Nextcloud\Artikel Cognitive Affective Maps Tools\CAM tools\CAMtools_CAMEL\static\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fenn\Nextcloud\Artikel Cognitive Affective Maps Tools\CAM tools\CAMtools_CAMEL\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86271E35-0185-4172-BC41-A70E75E1AE1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71CB72C-A50E-450A-8E5E-D00ADC64A3F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="536">
   <si>
     <t>english</t>
   </si>
@@ -334,9 +334,6 @@
     <t>Concepts support each other</t>
   </si>
   <si>
-    <t>Concepts inhibit each other</t>
-  </si>
-  <si>
     <t>qr_concept_10</t>
   </si>
   <si>
@@ -883,9 +880,6 @@
     <t>Mueva su Cognitive Affective Map</t>
   </si>
   <si>
-    <t>Support</t>
-  </si>
-  <si>
     <t>Inhibition</t>
   </si>
   <si>
@@ -1868,6 +1862,15 @@
   </si>
   <si>
     <t>Sie können Ihr CAM als Bild (svg-Datei) speichern.</t>
+  </si>
+  <si>
+    <t>Opposing</t>
+  </si>
+  <si>
+    <t>Supporting</t>
+  </si>
+  <si>
+    <t>Concepts oppose each other</t>
   </si>
 </sst>
 </file>
@@ -1935,7 +1938,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1948,6 +1951,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2248,8 +2257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2263,10 +2272,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -2281,10 +2290,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2292,48 +2301,48 @@
     </row>
     <row r="2" spans="1:9" ht="105">
       <c r="A2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="D3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="120">
@@ -2341,45 +2350,45 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60">
@@ -2393,16 +2402,16 @@
         <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2416,16 +2425,16 @@
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2439,16 +2448,16 @@
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2462,16 +2471,16 @@
         <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2485,16 +2494,16 @@
         <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="60">
@@ -2508,1833 +2517,1833 @@
         <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="G11" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30">
+      <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>456</v>
+      <c r="F13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30">
       <c r="A14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="60">
       <c r="A15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="105">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="60">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="G21" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="105">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="75">
       <c r="A23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="G23" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="G24" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="60">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>151</v>
-      </c>
       <c r="G26" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="105">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="G28" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="120">
       <c r="A29" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="75">
       <c r="A30" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>215</v>
-      </c>
       <c r="G30" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="60">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="45">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>170</v>
-      </c>
       <c r="G34" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="60">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="45">
       <c r="A36" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="60">
       <c r="A37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="G38" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="G39" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="G40" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30">
       <c r="A42" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="G42" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30">
       <c r="A43" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="G43" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30">
       <c r="A44" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="G44" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="G45" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="D46" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="G46" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30">
       <c r="A47" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="G47" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="G48" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>193</v>
-      </c>
       <c r="G49" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="G50" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30">
       <c r="A51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="D51" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>195</v>
-      </c>
       <c r="G51" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30">
       <c r="A52" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>238</v>
-      </c>
       <c r="G52" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="30">
+      <c r="A53" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="30">
+      <c r="A54" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="G54" s="4" t="s">
         <v>496</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="30">
-      <c r="A53" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="30">
-      <c r="A54" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30">
       <c r="A55" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="G55" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="30">
       <c r="A56" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="90">
       <c r="A57" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="30">
       <c r="A58" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="E58" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>225</v>
-      </c>
       <c r="G58" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="75">
       <c r="A59" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="30">
       <c r="A60" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="60">
       <c r="A61" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="30">
       <c r="A62" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="30">
       <c r="A63" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="75">
       <c r="A64" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="60">
       <c r="A65" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="75">
       <c r="A66" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="30">
       <c r="A67" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="45">
       <c r="A68" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="105">
       <c r="A69" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C69" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="E69" s="3" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="150">
       <c r="A70" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="60">
       <c r="A71" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="E71" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>533</v>
-      </c>
       <c r="F71" s="4" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="60">
       <c r="A72" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="30">
       <c r="A73" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>278</v>
-      </c>
       <c r="D73" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="30">
       <c r="A74" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="30">
       <c r="A75" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="30">
       <c r="A76" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="45">
       <c r="A77" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="60">
       <c r="A78" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="45">
       <c r="A79" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="45">
       <c r="A80" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>300</v>
-      </c>
       <c r="D80" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="45">
       <c r="A81" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="45">
       <c r="A82" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="45">
       <c r="A83" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="C83" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="150">
       <c r="A84" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C84" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="F84" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="G84" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="75">
       <c r="A85" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>314</v>
-      </c>
       <c r="C85" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="90">
       <c r="A86" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="D86" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>320</v>
-      </c>
       <c r="D87" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>321</v>
-      </c>
       <c r="D88" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D89" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F89" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E89" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="G89" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="30">
       <c r="A90" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="C90" s="2" t="s">
+      <c r="E90" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F90" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>362</v>
-      </c>
       <c r="G90" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>